<commit_message>
commit before data files change
</commit_message>
<xml_diff>
--- a/codebusters_data_analysis/My-JQL-Queries.xlsx
+++ b/codebusters_data_analysis/My-JQL-Queries.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MyProjects\PythonDataScience\codebusters_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7B9D2B-F5F9-482F-B02A-8E3F4BC0343C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A141FB-5872-4326-AD6F-A6CBC9FCEED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JQL" sheetId="1" r:id="rId1"/>
     <sheet name="Jira Api Query" sheetId="2" r:id="rId2"/>
     <sheet name="CSV" sheetId="5" r:id="rId3"/>
     <sheet name="InProgress" sheetId="3" r:id="rId4"/>
-    <sheet name="SLA" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="SLA" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Query</t>
   </si>
@@ -159,13 +160,16 @@
     <t>project = CI AND issuetype in (standardIssueTypes(), "Expense Delivery") AND "Epic Link" is EMPTY AND "Case Number/s" is not EMPTY AND cf[14125] in ("Service Request (SR)") AND labels in (Partners) AND resolved is not EMPTY AND resolutiondate &gt;= 2022-12-19</t>
   </si>
   <si>
-    <t>project = CI AND issuetype in (standardIssueTypes(), "Expense Delivery") AND "Epic Link" is EMPTY AND "Case Number/s" is not EMPTY AND cf[14125] in (Incident Request (IR)") AND resolved is not EMPTY AND resolutiondate &gt;= 2022-12-19</t>
-  </si>
-  <si>
-    <t>project = CI AND  issuetype  in ("Expense Delivery", "Internal Task" ) AND createdDate &gt;= 2022-12-19 AND createdDate  &lt;= 2023-03-24</t>
-  </si>
-  <si>
     <t>Individual Tasks</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>project = CI AND issuetype in (standardIssueTypes(), "Expense Delivery") AND "Epic Link" is EMPTY AND "Case Number/s" is not EMPTY AND cf[14125] in ("Incident Request (IR)") AND resolved is not EMPTY AND resolutiondate &gt;= 2022-12-19</t>
+  </si>
+  <si>
+    <t>project = CI AND  type = "Individual Task" AND resolveDate &gt;= 2023-07-03 AND resolveDate  &lt;= 2023-08-17</t>
   </si>
 </sst>
 </file>
@@ -544,13 +548,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="86.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -558,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -566,7 +570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -595,13 +599,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="122.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="122.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -609,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -617,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -625,12 +629,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -652,27 +656,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE1746A-6AF8-4BED-B32A-18821223FBA7}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="102.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="102.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -680,7 +684,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -688,11 +692,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -710,16 +719,16 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="93.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -727,7 +736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -735,7 +744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -743,7 +752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -751,7 +760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -759,7 +768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -767,7 +776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -775,12 +784,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -788,7 +797,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -796,7 +805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -815,6 +824,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EA9161-7662-4E49-81AB-581705F267A5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;KFF8C00CONFIDENTIAL &amp; RESTRICTED&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673CF551-303E-4C50-A3A8-3198BAFD63DD}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -822,22 +847,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="155.109375" customWidth="1"/>
+    <col min="1" max="1" width="155.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>

</xml_diff>